<commit_message>
updated time.clock() to be time.perf_counter() in all scripts
</commit_message>
<xml_diff>
--- a/ppa/Input_Template/XLSX/PPA_Template_ArterialExp.xlsx
+++ b/ppa/Input_Template/XLSX/PPA_Template_ArterialExp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\ProjectLevelPerformanceAssessment\PPAv2\PPA2_0_code\PPA2\Input_Template\XLSX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dconly\GitRepos\PPA2\ppa\Input_Template\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808729FF-1413-45C0-8BB8-02B4EEB7514A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6358AE1-9404-4615-A536-C92E0CE49E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="712" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11970" yWindow="195" windowWidth="24255" windowHeight="14970" tabRatio="712" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0ATitlePg" sheetId="4" r:id="rId1"/>
@@ -19763,7 +19763,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26035,7 +26035,7 @@
   <dimension ref="A1:H66"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26144,8 +26144,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView view="pageLayout" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26371,7 +26371,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView view="pageLayout" topLeftCell="A93" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26595,8 +26597,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView view="pageLayout" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26753,7 +26755,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A44" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
@@ -26905,7 +26907,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
@@ -27066,7 +27068,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>